<commit_message>
korjasin sprintit ja tarkistin paikkansapitävyyden
Sprintit oli merkattu 1 vko pituisiksi, vaikka ne on 2 vkoa oikeasti.
</commit_message>
<xml_diff>
--- a/GitGud_Backlog.xlsx
+++ b/GitGud_Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Sprintti 1</t>
   </si>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>Kyselyn kysymykset voi hakea JSON:lla</t>
-  </si>
-  <si>
-    <t>Sprintti 4</t>
-  </si>
-  <si>
-    <t>Sprintti 5</t>
   </si>
   <si>
     <t>20.11-22.11.2017</t>
@@ -331,9 +325,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,24 +355,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -678,7 +672,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B11" sqref="B11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,322 +684,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
       <c r="H3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
       <c r="H4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="22" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="23"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="23"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B10:G10"/>
@@ -1015,14 +1009,14 @@
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>